<commit_message>
Stabilize upload flow, add structured OCR & payment analytics, fix redirects
</commit_message>
<xml_diff>
--- a/data/output/payments.xlsx
+++ b/data/output/payments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,42 +441,74 @@
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
+          <t>invoice_no</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>amount_detected</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>currency</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>signature_present</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>ink_fraction</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>amount</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>payable</t>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>fraud_risk_score</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>final_status</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>processed_utc</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>sample1.png</t>
-        </is>
-      </c>
-      <c r="B2" t="b">
-        <v>1</v>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>IOCL-2024-INV-001</t>
+        </is>
       </c>
       <c r="C2" t="n">
-        <v>0.5249</v>
-      </c>
-      <c r="D2" t="n">
         <v>1000</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>INR</t>
+        </is>
       </c>
       <c r="E2" t="b">
         <v>1</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>APPROVED</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2025-12-17 08:36:40</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor to agentic architecture, add executive dashboard, UI integration, and audit-safe pipeline
</commit_message>
<xml_diff>
--- a/data/output/payments.xlsx
+++ b/data/output/payments.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,7 +440,7 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>file</t>
+          <t>file_name</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
@@ -472,6 +476,31 @@
       <c r="H1" s="1" t="inlineStr">
         <is>
           <t>processed_utc</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>ink_density_score</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>avg_ocr_confidence</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>audit_remarks</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>decision_stage</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>data_quality_flag</t>
         </is>
       </c>
     </row>
@@ -483,7 +512,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>IOCL-2024-INV-001</t>
+          <t>AUTO-DETECTED</t>
         </is>
       </c>
       <c r="C2" t="n">
@@ -505,9 +534,165 @@
           <t>APPROVED</t>
         </is>
       </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>2025-12-17 08:36:40</t>
+      <c r="H2" s="2" t="n">
+        <v>46009.45200974537</v>
+      </c>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="n">
+        <v>642</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>INR</t>
+        </is>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>ON_HOLD</t>
+        </is>
+      </c>
+      <c r="H3" s="2" t="n">
+        <v>46015.3009153588</v>
+      </c>
+      <c r="I3" t="n">
+        <v>0.1215</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0.174</v>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>Low OCR confidence</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>REQUIRES_MANUAL_REVIEW</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>LOW_CONFIDENCE</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="n">
+        <v>642</v>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>INR</t>
+        </is>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>ON_HOLD</t>
+        </is>
+      </c>
+      <c r="H4" s="2" t="n">
+        <v>46015.30579377315</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0.1215</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0.174</v>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>Low OCR confidence</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>REQUIRES_MANUAL_REVIEW</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>LOW_CONFIDENCE</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>sample1.PNG</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr"/>
+      <c r="C5" t="n">
+        <v>642</v>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>INR</t>
+        </is>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>ON_HOLD</t>
+        </is>
+      </c>
+      <c r="H5" s="2" t="n">
+        <v>46015.30790904717</v>
+      </c>
+      <c r="I5" t="n">
+        <v>0.1215</v>
+      </c>
+      <c r="J5" t="n">
+        <v>0.174</v>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>Low OCR confidence</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>REQUIRES_MANUAL_REVIEW</t>
+        </is>
+      </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>LOW_CONFIDENCE</t>
         </is>
       </c>
     </row>

</xml_diff>